<commit_message>
done with project lab 1
</commit_message>
<xml_diff>
--- a/FinalProject/Budget.xlsx
+++ b/FinalProject/Budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkans\OneDrive\Desktop\stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dirkt\Documents\School\projectLab1\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDFFFA3-23DD-4BAC-A11D-C8EA04DD53EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65740DD-6810-41A3-959F-98DE284D13C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8BB2A8C5-712E-4190-8588-7F5E0E3A700D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{8BB2A8C5-712E-4190-8588-7F5E0E3A700D}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Budget" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="91">
   <si>
     <t>Project Lab 1</t>
   </si>
@@ -551,6 +551,7 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -593,7 +594,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2AB47C0-B6FA-4FC5-84F1-E15593E5DB37}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -926,16 +926,16 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="40" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
@@ -990,7 +990,7 @@
       <c r="G4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="52"/>
+      <c r="I4" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1001,11 +1001,11 @@
       </c>
       <c r="C5" s="4">
         <f>'Labor Hours'!J2</f>
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="D5" s="16">
         <f>B5*C5</f>
-        <v>1275</v>
+        <v>1920</v>
       </c>
       <c r="E5" s="6">
         <v>15</v>
@@ -1033,11 +1033,11 @@
       </c>
       <c r="C6" s="4">
         <f>'Labor Hours'!J3</f>
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="D6" s="16">
         <f>B6*C6</f>
-        <v>1140</v>
+        <v>1380</v>
       </c>
       <c r="E6" s="6">
         <v>15</v>
@@ -1094,7 +1094,7 @@
       </c>
       <c r="D9" s="16">
         <f>SUM(D5:D7)</f>
-        <v>3525</v>
+        <v>4410</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="4" t="s">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="D10" s="17">
         <f>D9</f>
-        <v>3525</v>
+        <v>4410</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>16</v>
@@ -1138,7 +1138,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="18">
         <f>SUM(D9:D10)</f>
-        <v>7050</v>
+        <v>8820</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="4"/>
@@ -1146,10 +1146,10 @@
         <f>SUM(G9:G10)</f>
         <v>14400</v>
       </c>
-      <c r="I11" s="42" t="s">
+      <c r="I11" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="J11" s="42"/>
+      <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
@@ -1158,10 +1158,10 @@
       <c r="E12" s="6"/>
       <c r="F12" s="4"/>
       <c r="G12" s="7"/>
-      <c r="I12" s="43" t="s">
+      <c r="I12" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="44"/>
+      <c r="J12" s="45"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -1173,10 +1173,10 @@
       <c r="E13" s="6"/>
       <c r="F13" s="4"/>
       <c r="G13" s="7"/>
-      <c r="I13" s="45" t="s">
+      <c r="I13" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="46"/>
+      <c r="J13" s="47"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1203,10 +1203,10 @@
         <f>E14*F14</f>
         <v>600</v>
       </c>
-      <c r="I14" s="47" t="s">
+      <c r="I14" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="48"/>
+      <c r="J14" s="49"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1358,14 +1358,14 @@
         <v>29</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="41" t="s">
+      <c r="H23" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41" t="s">
+      <c r="I23" s="42"/>
+      <c r="J23" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="K23" s="41"/>
+      <c r="K23" s="42"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -1392,14 +1392,14 @@
         <f>E24*F24*J24</f>
         <v>26.999400000000001</v>
       </c>
-      <c r="H24" s="41">
+      <c r="H24" s="42">
         <v>18</v>
       </c>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41">
+      <c r="I24" s="42"/>
+      <c r="J24" s="42">
         <v>30</v>
       </c>
-      <c r="K24" s="41"/>
+      <c r="K24" s="42"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -1513,7 +1513,7 @@
       <c r="C30" s="4"/>
       <c r="D30" s="19">
         <f>SUM(D11,D17,D21,D28)</f>
-        <v>7948.8689199999999</v>
+        <v>9718.8689200000008</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="4"/>
@@ -1532,7 +1532,7 @@
       </c>
       <c r="D31" s="17">
         <f>D30*C31</f>
-        <v>4371.8779060000006</v>
+        <v>5345.3779060000006</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="9">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="D32" s="19">
         <f>SUM(D30:D31)</f>
-        <v>12320.746826000001</v>
+        <v>15064.246826000002</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="15" t="s">
@@ -1587,10 +1587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7020275-B2DA-4DA8-8538-10FD245A3C38}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection sqref="A1:J61"/>
+      <selection activeCell="I74" sqref="A1:J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1620,10 +1620,10 @@
       <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="49"/>
+      <c r="J1" s="50"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="20">
@@ -1654,8 +1654,8 @@
         <v>10</v>
       </c>
       <c r="J2" s="23">
-        <f>SUM(B2:B61)</f>
-        <v>85</v>
+        <f>SUM(B2:B74)</f>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1687,8 +1687,8 @@
         <v>43</v>
       </c>
       <c r="J3" s="23">
-        <f>SUM(C2:C61)</f>
-        <v>76</v>
+        <f>SUM(C2:C74)</f>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1720,7 +1720,7 @@
         <v>44</v>
       </c>
       <c r="J4" s="23">
-        <f>SUM(D2:D61)</f>
+        <f>SUM(D2:D74)</f>
         <v>74</v>
       </c>
     </row>
@@ -1926,10 +1926,10 @@
       <c r="H11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="50" t="s">
+      <c r="I11" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="J11" s="41"/>
+      <c r="J11" s="42"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="20">
@@ -1956,10 +1956,10 @@
       <c r="H12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I12" s="51" t="s">
+      <c r="I12" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="J12" s="49"/>
+      <c r="J12" s="50"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="20">
@@ -3006,13 +3006,13 @@
         <v>44663</v>
       </c>
       <c r="B53" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C53" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D53" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E53" s="2">
         <v>0</v>
@@ -3029,24 +3029,24 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="20">
-        <v>44663</v>
-      </c>
-      <c r="B54" s="36">
-        <v>0</v>
-      </c>
-      <c r="C54" s="36">
-        <v>0</v>
-      </c>
-      <c r="D54" s="36">
-        <v>0</v>
-      </c>
-      <c r="E54" s="36">
-        <v>0</v>
-      </c>
-      <c r="F54" s="36">
-        <v>0</v>
-      </c>
-      <c r="G54" s="36">
+        <v>44664</v>
+      </c>
+      <c r="B54" s="2">
+        <v>0</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0</v>
+      </c>
+      <c r="E54" s="2">
+        <v>0</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0</v>
+      </c>
+      <c r="G54" s="2">
         <v>0</v>
       </c>
       <c r="H54" s="36" t="s">
@@ -3055,24 +3055,24 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="20">
-        <v>44663</v>
-      </c>
-      <c r="B55" s="36">
-        <v>0</v>
-      </c>
-      <c r="C55" s="36">
-        <v>0</v>
-      </c>
-      <c r="D55" s="36">
-        <v>0</v>
-      </c>
-      <c r="E55" s="36">
-        <v>0</v>
-      </c>
-      <c r="F55" s="36">
-        <v>0</v>
-      </c>
-      <c r="G55" s="36">
+        <v>44665</v>
+      </c>
+      <c r="B55" s="2">
+        <v>0</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0</v>
+      </c>
+      <c r="E55" s="2">
+        <v>0</v>
+      </c>
+      <c r="F55" s="2">
+        <v>0</v>
+      </c>
+      <c r="G55" s="2">
         <v>0</v>
       </c>
       <c r="H55" s="36" t="s">
@@ -3081,24 +3081,24 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="20">
-        <v>44663</v>
-      </c>
-      <c r="B56" s="36">
-        <v>0</v>
-      </c>
-      <c r="C56" s="36">
-        <v>0</v>
-      </c>
-      <c r="D56" s="36">
+        <v>44666</v>
+      </c>
+      <c r="B56" s="2">
+        <v>0</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0</v>
+      </c>
+      <c r="D56" s="2">
         <v>0</v>
       </c>
       <c r="E56" s="2">
         <v>0</v>
       </c>
-      <c r="F56" s="36">
-        <v>0</v>
-      </c>
-      <c r="G56" s="36">
+      <c r="F56" s="2">
+        <v>0</v>
+      </c>
+      <c r="G56" s="2">
         <v>0</v>
       </c>
       <c r="H56" s="36" t="s">
@@ -3107,24 +3107,24 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="20">
-        <v>44663</v>
-      </c>
-      <c r="B57" s="36">
-        <v>1</v>
-      </c>
-      <c r="C57" s="36">
-        <v>0</v>
-      </c>
-      <c r="D57" s="36">
+        <v>44667</v>
+      </c>
+      <c r="B57" s="2">
+        <v>0</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0</v>
+      </c>
+      <c r="D57" s="2">
         <v>0</v>
       </c>
       <c r="E57" s="2">
         <v>0</v>
       </c>
-      <c r="F57" s="36">
-        <v>0</v>
-      </c>
-      <c r="G57" s="36">
+      <c r="F57" s="2">
+        <v>0</v>
+      </c>
+      <c r="G57" s="2">
         <v>0</v>
       </c>
       <c r="H57" s="36" t="s">
@@ -3133,24 +3133,24 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="20">
-        <v>44663</v>
-      </c>
-      <c r="B58" s="36">
-        <v>0</v>
-      </c>
-      <c r="C58" s="36">
-        <v>0</v>
-      </c>
-      <c r="D58" s="36">
+        <v>44668</v>
+      </c>
+      <c r="B58" s="2">
+        <v>0</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0</v>
+      </c>
+      <c r="D58" s="2">
         <v>0</v>
       </c>
       <c r="E58" s="2">
         <v>0</v>
       </c>
-      <c r="F58" s="36">
-        <v>0</v>
-      </c>
-      <c r="G58" s="36">
+      <c r="F58" s="2">
+        <v>0</v>
+      </c>
+      <c r="G58" s="2">
         <v>0</v>
       </c>
       <c r="H58" s="36" t="s">
@@ -3159,24 +3159,24 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="20">
-        <v>44663</v>
-      </c>
-      <c r="B59" s="36">
+        <v>44669</v>
+      </c>
+      <c r="B59" s="2">
         <v>0</v>
       </c>
       <c r="C59" s="2">
         <v>0</v>
       </c>
-      <c r="D59" s="36">
+      <c r="D59" s="2">
         <v>0</v>
       </c>
       <c r="E59" s="2">
         <v>0</v>
       </c>
-      <c r="F59" s="36">
-        <v>0</v>
-      </c>
-      <c r="G59" s="36">
+      <c r="F59" s="2">
+        <v>0</v>
+      </c>
+      <c r="G59" s="2">
         <v>0</v>
       </c>
       <c r="H59" s="36" t="s">
@@ -3185,24 +3185,24 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="20">
-        <v>44663</v>
-      </c>
-      <c r="B60" s="36">
-        <v>3</v>
+        <v>44670</v>
+      </c>
+      <c r="B60" s="2">
+        <v>0</v>
       </c>
       <c r="C60" s="2">
-        <v>3</v>
-      </c>
-      <c r="D60" s="36">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0</v>
       </c>
       <c r="E60" s="2">
         <v>0</v>
       </c>
-      <c r="F60" s="36">
-        <v>0</v>
-      </c>
-      <c r="G60" s="36">
+      <c r="F60" s="2">
+        <v>0</v>
+      </c>
+      <c r="G60" s="2">
         <v>0</v>
       </c>
       <c r="H60" s="36" t="s">
@@ -3211,28 +3211,366 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="20">
-        <v>44663</v>
-      </c>
-      <c r="B61" s="36">
-        <v>3</v>
+        <v>44671</v>
+      </c>
+      <c r="B61" s="2">
+        <v>0</v>
       </c>
       <c r="C61" s="2">
-        <v>3</v>
-      </c>
-      <c r="D61" s="36">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0</v>
       </c>
       <c r="E61" s="2">
         <v>0</v>
       </c>
-      <c r="F61" s="36">
-        <v>0</v>
-      </c>
-      <c r="G61" s="36">
+      <c r="F61" s="2">
+        <v>0</v>
+      </c>
+      <c r="G61" s="2">
         <v>0</v>
       </c>
       <c r="H61" s="36" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="20">
+        <v>44672</v>
+      </c>
+      <c r="B62" s="2">
+        <v>0</v>
+      </c>
+      <c r="C62" s="2">
+        <v>0</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0</v>
+      </c>
+      <c r="E62" s="2">
+        <v>0</v>
+      </c>
+      <c r="F62" s="2">
+        <v>0</v>
+      </c>
+      <c r="G62" s="2">
+        <v>0</v>
+      </c>
+      <c r="H62" s="36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="20">
+        <v>44673</v>
+      </c>
+      <c r="B63" s="2">
+        <v>0</v>
+      </c>
+      <c r="C63" s="2">
+        <v>0</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0</v>
+      </c>
+      <c r="F63" s="2">
+        <v>0</v>
+      </c>
+      <c r="G63" s="2">
+        <v>0</v>
+      </c>
+      <c r="H63" s="36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" s="20">
+        <v>44674</v>
+      </c>
+      <c r="B64" s="2">
+        <v>0</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0</v>
+      </c>
+      <c r="D64" s="2">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2">
+        <v>0</v>
+      </c>
+      <c r="F64" s="2">
+        <v>0</v>
+      </c>
+      <c r="G64" s="2">
+        <v>0</v>
+      </c>
+      <c r="H64" s="36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" s="20">
+        <v>44675</v>
+      </c>
+      <c r="B65" s="2">
+        <v>0</v>
+      </c>
+      <c r="C65" s="2">
+        <v>0</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0</v>
+      </c>
+      <c r="E65" s="2">
+        <v>0</v>
+      </c>
+      <c r="F65" s="2">
+        <v>0</v>
+      </c>
+      <c r="G65" s="2">
+        <v>0</v>
+      </c>
+      <c r="H65" s="36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="20">
+        <v>44676</v>
+      </c>
+      <c r="B66" s="2">
+        <v>5</v>
+      </c>
+      <c r="C66" s="2">
+        <v>0</v>
+      </c>
+      <c r="D66" s="2">
+        <v>0</v>
+      </c>
+      <c r="E66" s="2">
+        <v>0</v>
+      </c>
+      <c r="F66" s="2">
+        <v>0</v>
+      </c>
+      <c r="G66" s="2">
+        <v>0</v>
+      </c>
+      <c r="H66" s="36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" s="20">
+        <v>44677</v>
+      </c>
+      <c r="B67" s="2">
+        <v>10</v>
+      </c>
+      <c r="C67" s="2">
+        <v>0</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2">
+        <v>0</v>
+      </c>
+      <c r="F67" s="2">
+        <v>0</v>
+      </c>
+      <c r="G67" s="2">
+        <v>0</v>
+      </c>
+      <c r="H67" s="36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" s="20">
+        <v>44678</v>
+      </c>
+      <c r="B68" s="2">
+        <v>12</v>
+      </c>
+      <c r="C68" s="2">
+        <v>12</v>
+      </c>
+      <c r="D68" s="2">
+        <v>0</v>
+      </c>
+      <c r="E68" s="2">
+        <v>0</v>
+      </c>
+      <c r="F68" s="2">
+        <v>0</v>
+      </c>
+      <c r="G68" s="2">
+        <v>0</v>
+      </c>
+      <c r="H68" s="36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" s="20">
+        <v>44679</v>
+      </c>
+      <c r="B69" s="2">
+        <v>6</v>
+      </c>
+      <c r="C69" s="2">
+        <v>4</v>
+      </c>
+      <c r="D69" s="2">
+        <v>4</v>
+      </c>
+      <c r="E69" s="2">
+        <v>0</v>
+      </c>
+      <c r="F69" s="2">
+        <v>0</v>
+      </c>
+      <c r="G69" s="2">
+        <v>0</v>
+      </c>
+      <c r="H69" s="36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="20">
+        <v>44680</v>
+      </c>
+      <c r="B70" s="2">
+        <v>8</v>
+      </c>
+      <c r="C70" s="2">
+        <v>0</v>
+      </c>
+      <c r="D70" s="2">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2">
+        <v>0</v>
+      </c>
+      <c r="F70" s="2">
+        <v>0</v>
+      </c>
+      <c r="G70" s="2">
+        <v>0</v>
+      </c>
+      <c r="H70" s="36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="20">
+        <v>44681</v>
+      </c>
+      <c r="B71" s="2">
+        <v>12</v>
+      </c>
+      <c r="C71" s="2">
+        <v>8</v>
+      </c>
+      <c r="D71" s="2">
+        <v>4</v>
+      </c>
+      <c r="E71" s="2">
+        <v>0</v>
+      </c>
+      <c r="F71" s="2">
+        <v>0</v>
+      </c>
+      <c r="G71" s="2">
+        <v>0</v>
+      </c>
+      <c r="H71" s="36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" s="20">
+        <v>44682</v>
+      </c>
+      <c r="B72" s="2">
+        <v>0</v>
+      </c>
+      <c r="C72" s="2">
+        <v>0</v>
+      </c>
+      <c r="D72" s="2">
+        <v>0</v>
+      </c>
+      <c r="E72" s="2">
+        <v>0</v>
+      </c>
+      <c r="F72" s="2">
+        <v>0</v>
+      </c>
+      <c r="G72" s="2">
+        <v>0</v>
+      </c>
+      <c r="H72" s="36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" s="20">
+        <v>44683</v>
+      </c>
+      <c r="B73" s="2">
+        <v>0</v>
+      </c>
+      <c r="C73" s="2">
+        <v>0</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0</v>
+      </c>
+      <c r="E73" s="2">
+        <v>0</v>
+      </c>
+      <c r="F73" s="2">
+        <v>0</v>
+      </c>
+      <c r="G73" s="2">
+        <v>0</v>
+      </c>
+      <c r="H73" s="36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" s="20">
+        <v>44684</v>
+      </c>
+      <c r="B74" s="2">
+        <v>0</v>
+      </c>
+      <c r="C74" s="2">
+        <v>0</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0</v>
+      </c>
+      <c r="E74" s="2">
+        <v>0</v>
+      </c>
+      <c r="F74" s="2">
+        <v>0</v>
+      </c>
+      <c r="G74" s="2">
+        <v>0</v>
+      </c>
+      <c r="H74" s="36" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -3250,7 +3588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9B8CE2-A2E2-43AC-883D-24385E4073B8}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:G26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Final Budget with the bill of materials
</commit_message>
<xml_diff>
--- a/FinalProject/Budget.xlsx
+++ b/FinalProject/Budget.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkans\OneDrive\Desktop\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D4994D-CA6F-4B86-9766-A9B776AEDF88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9312B5FA-716A-4E2B-A810-EA8D11EF991F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8BB2A8C5-712E-4190-8588-7F5E0E3A700D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{8BB2A8C5-712E-4190-8588-7F5E0E3A700D}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Budget" sheetId="1" r:id="rId1"/>
     <sheet name="Labor Hours" sheetId="2" r:id="rId2"/>
     <sheet name="Material Costs" sheetId="3" r:id="rId3"/>
+    <sheet name="Bill Of Materials" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="94">
   <si>
     <t>Project Lab 1</t>
   </si>
@@ -50,9 +51,6 @@
     <t>Start Date</t>
   </si>
   <si>
-    <t>Today</t>
-  </si>
-  <si>
     <t>End Date</t>
   </si>
   <si>
@@ -309,6 +307,18 @@
   </si>
   <si>
     <t xml:space="preserve">Screw terminals </t>
+  </si>
+  <si>
+    <t>Phototransistors (2)</t>
+  </si>
+  <si>
+    <t>Infrared Sensors (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servo Motors </t>
   </si>
 </sst>
 </file>
@@ -349,7 +359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +381,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -506,7 +522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -530,7 +546,6 @@
     <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -552,6 +567,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -594,6 +615,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -911,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2AB47C0-B6FA-4FC5-84F1-E15593E5DB37}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -926,16 +948,16 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="41" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
@@ -953,7 +975,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="4"/>
@@ -961,40 +983,36 @@
       <c r="E3" s="6"/>
       <c r="F3" s="4"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="21">
-        <v>44671</v>
-      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="54"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="E4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="38"/>
+      <c r="I4" s="37"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="6">
         <v>15</v>
@@ -1018,15 +1036,15 @@
         <v>2400</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="22">
+        <v>4</v>
+      </c>
+      <c r="I5" s="21">
         <v>44687</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="6">
         <v>15</v>
@@ -1052,7 +1070,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="6">
         <v>15</v>
@@ -1086,11 +1104,11 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="16">
         <f>SUM(D5:D7)</f>
@@ -1098,7 +1116,7 @@
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G9" s="8">
         <f>SUM(G5:G7)</f>
@@ -1107,10 +1125,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="9">
         <v>1</v>
@@ -1120,7 +1138,7 @@
         <v>3240</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="9">
         <v>1</v>
@@ -1132,7 +1150,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
@@ -1146,10 +1164,10 @@
         <f>SUM(G9:G10)</f>
         <v>14400</v>
       </c>
-      <c r="I11" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="43"/>
+      <c r="I11" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="44"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
@@ -1158,14 +1176,14 @@
       <c r="E12" s="6"/>
       <c r="F12" s="4"/>
       <c r="G12" s="7"/>
-      <c r="I12" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="J12" s="45"/>
+      <c r="I12" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="46"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
@@ -1173,14 +1191,14 @@
       <c r="E13" s="6"/>
       <c r="F13" s="4"/>
       <c r="G13" s="7"/>
-      <c r="I13" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="47"/>
+      <c r="I13" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="48"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="6">
         <v>40</v>
@@ -1203,14 +1221,14 @@
         <f>E14*F14</f>
         <v>600</v>
       </c>
-      <c r="I14" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="J14" s="49"/>
+      <c r="I14" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="50"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="6">
         <v>15</v>
@@ -1238,7 +1256,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="6">
         <v>200</v>
@@ -1264,7 +1282,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="4"/>
@@ -1289,7 +1307,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="4"/>
@@ -1306,7 +1324,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="4"/>
@@ -1317,7 +1335,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="4"/>
@@ -1342,34 +1360,34 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="42" t="s">
+      <c r="H23" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="K23" s="42"/>
+      <c r="K23" s="43"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="12">
         <f>449.99</f>
@@ -1382,7 +1400,7 @@
         <f>B24*C24*H24</f>
         <v>16.199639999999999</v>
       </c>
-      <c r="E24" s="34">
+      <c r="E24" s="33">
         <v>449.99</v>
       </c>
       <c r="F24" s="13">
@@ -1392,18 +1410,18 @@
         <f>E24*F24*J24</f>
         <v>26.999400000000001</v>
       </c>
-      <c r="H24" s="42">
+      <c r="H24" s="43">
         <v>18</v>
       </c>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42">
+      <c r="I24" s="43"/>
+      <c r="J24" s="43">
         <v>30</v>
       </c>
-      <c r="K24" s="42"/>
+      <c r="K24" s="43"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="12">
         <f>415</f>
@@ -1416,7 +1434,7 @@
         <f>B25*C25*H24</f>
         <v>14.940000000000001</v>
       </c>
-      <c r="E25" s="34">
+      <c r="E25" s="33">
         <v>415</v>
       </c>
       <c r="F25" s="13">
@@ -1429,23 +1447,23 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B26" s="12">
         <f>99.99</f>
         <v>99.99</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="31">
         <v>2E-3</v>
       </c>
       <c r="D26" s="10">
         <f>B26*C26*H24</f>
         <v>3.59964</v>
       </c>
-      <c r="E26" s="35">
+      <c r="E26" s="34">
         <v>99</v>
       </c>
-      <c r="F26" s="32">
+      <c r="F26" s="31">
         <v>2E-3</v>
       </c>
       <c r="G26" s="7">
@@ -1455,7 +1473,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" s="12">
         <f>99.99</f>
@@ -1464,25 +1482,25 @@
       <c r="C27" s="13">
         <v>2E-3</v>
       </c>
-      <c r="D27" s="30">
+      <c r="D27" s="29">
         <f>B27*C27*H24</f>
         <v>3.59964</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="32">
         <f>99</f>
         <v>99</v>
       </c>
       <c r="F27" s="13">
         <v>2E-3</v>
       </c>
-      <c r="G27" s="31">
+      <c r="G27" s="30">
         <f>E27*F27*J24</f>
         <v>5.94</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="4"/>
@@ -1507,7 +1525,7 @@
     </row>
     <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="4"/>
@@ -1524,7 +1542,7 @@
     </row>
     <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="9">
@@ -1545,11 +1563,11 @@
     </row>
     <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" s="14"/>
       <c r="C32" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" s="19">
         <f>SUM(D30:D31)</f>
@@ -1557,7 +1575,7 @@
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G32" s="5">
         <f>SUM(G30:G31)</f>
@@ -1589,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7020275-B2DA-4DA8-8538-10FD245A3C38}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L69" sqref="L69"/>
+    <sheetView topLeftCell="A3" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AA32" sqref="AA32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1600,30 +1618,30 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="50"/>
+      <c r="J1" s="51"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="20">
@@ -1648,12 +1666,12 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="23">
+        <v>48</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="22">
         <f>SUM(B2:B53)</f>
         <v>78</v>
       </c>
@@ -1681,12 +1699,12 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="23">
+        <v>49</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="22">
         <f>SUM(C2:C53)</f>
         <v>70</v>
       </c>
@@ -1714,12 +1732,12 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" s="23">
+        <v>50</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="22">
         <f>SUM(D2:D53)</f>
         <v>68</v>
       </c>
@@ -1743,16 +1761,16 @@
       <c r="F5" s="2">
         <v>0</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="23">
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="23">
+        <v>51</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="22">
         <f>SUM(E2:E53)</f>
         <v>0</v>
       </c>
@@ -1780,12 +1798,12 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="23">
+        <v>52</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="22">
         <f>SUM(F2:F53)</f>
         <v>1</v>
       </c>
@@ -1813,12 +1831,12 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="23">
+        <v>46</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="22">
         <f>SUM(G2:G53)</f>
         <v>2</v>
       </c>
@@ -1846,7 +1864,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1872,7 +1890,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1898,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1924,12 +1942,12 @@
         <v>0</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="42"/>
+        <v>50</v>
+      </c>
+      <c r="I11" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="20">
@@ -1954,12 +1972,12 @@
         <v>0</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I12" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="50"/>
+        <v>51</v>
+      </c>
+      <c r="I12" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" s="51"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="20">
@@ -1984,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -2010,7 +2028,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -2036,7 +2054,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -2062,7 +2080,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -2088,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -2114,7 +2132,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -2140,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -2166,7 +2184,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -2192,7 +2210,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -2218,7 +2236,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -2244,7 +2262,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -2270,7 +2288,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -2296,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2322,7 +2340,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -2348,7 +2366,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -2374,7 +2392,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -2400,7 +2418,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -2426,59 +2444,59 @@
         <v>0</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="20">
         <v>44641</v>
       </c>
-      <c r="B31" s="36">
+      <c r="B31" s="35">
         <v>4</v>
       </c>
-      <c r="C31" s="36">
-        <v>0</v>
-      </c>
-      <c r="D31" s="36">
-        <v>0</v>
-      </c>
-      <c r="E31" s="36">
-        <v>0</v>
-      </c>
-      <c r="F31" s="36">
-        <v>0</v>
-      </c>
-      <c r="G31" s="36">
-        <v>0</v>
-      </c>
-      <c r="H31" s="36" t="s">
-        <v>52</v>
+      <c r="C31" s="35">
+        <v>0</v>
+      </c>
+      <c r="D31" s="35">
+        <v>0</v>
+      </c>
+      <c r="E31" s="35">
+        <v>0</v>
+      </c>
+      <c r="F31" s="35">
+        <v>0</v>
+      </c>
+      <c r="G31" s="35">
+        <v>0</v>
+      </c>
+      <c r="H31" s="35" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="20">
         <v>44642</v>
       </c>
-      <c r="B32" s="36">
-        <v>3</v>
-      </c>
-      <c r="C32" s="36">
-        <v>3</v>
-      </c>
-      <c r="D32" s="36">
-        <v>3</v>
-      </c>
-      <c r="E32" s="36">
-        <v>0</v>
-      </c>
-      <c r="F32" s="36">
-        <v>0</v>
-      </c>
-      <c r="G32" s="36">
-        <v>0</v>
-      </c>
-      <c r="H32" s="36" t="s">
-        <v>53</v>
+      <c r="B32" s="35">
+        <v>3</v>
+      </c>
+      <c r="C32" s="35">
+        <v>3</v>
+      </c>
+      <c r="D32" s="35">
+        <v>3</v>
+      </c>
+      <c r="E32" s="35">
+        <v>0</v>
+      </c>
+      <c r="F32" s="35">
+        <v>0</v>
+      </c>
+      <c r="G32" s="35">
+        <v>0</v>
+      </c>
+      <c r="H32" s="35" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -2503,8 +2521,8 @@
       <c r="G33" s="2">
         <v>0</v>
       </c>
-      <c r="H33" s="36" t="s">
-        <v>47</v>
+      <c r="H33" s="35" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -2529,8 +2547,8 @@
       <c r="G34" s="2">
         <v>0</v>
       </c>
-      <c r="H34" s="36" t="s">
-        <v>48</v>
+      <c r="H34" s="35" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -2555,8 +2573,8 @@
       <c r="G35" s="2">
         <v>0</v>
       </c>
-      <c r="H35" s="36" t="s">
-        <v>49</v>
+      <c r="H35" s="35" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -2581,8 +2599,8 @@
       <c r="G36" s="2">
         <v>0</v>
       </c>
-      <c r="H36" s="36" t="s">
-        <v>50</v>
+      <c r="H36" s="35" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -2607,8 +2625,8 @@
       <c r="G37" s="2">
         <v>0</v>
       </c>
-      <c r="H37" s="36" t="s">
-        <v>51</v>
+      <c r="H37" s="35" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -2633,8 +2651,8 @@
       <c r="G38" s="2">
         <v>0</v>
       </c>
-      <c r="H38" s="36" t="s">
-        <v>52</v>
+      <c r="H38" s="35" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -2659,8 +2677,8 @@
       <c r="G39" s="2">
         <v>2</v>
       </c>
-      <c r="H39" s="36" t="s">
-        <v>53</v>
+      <c r="H39" s="35" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -2685,8 +2703,8 @@
       <c r="G40" s="2">
         <v>0</v>
       </c>
-      <c r="H40" s="36" t="s">
-        <v>47</v>
+      <c r="H40" s="35" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -2711,8 +2729,8 @@
       <c r="G41" s="2">
         <v>0</v>
       </c>
-      <c r="H41" s="36" t="s">
-        <v>48</v>
+      <c r="H41" s="35" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -2737,8 +2755,8 @@
       <c r="G42" s="2">
         <v>0</v>
       </c>
-      <c r="H42" s="36" t="s">
-        <v>49</v>
+      <c r="H42" s="35" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -2763,8 +2781,8 @@
       <c r="G43" s="2">
         <v>0</v>
       </c>
-      <c r="H43" s="36" t="s">
-        <v>50</v>
+      <c r="H43" s="35" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -2789,8 +2807,8 @@
       <c r="G44" s="2">
         <v>0</v>
       </c>
-      <c r="H44" s="36" t="s">
-        <v>51</v>
+      <c r="H44" s="35" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -2815,8 +2833,8 @@
       <c r="G45" s="2">
         <v>0</v>
       </c>
-      <c r="H45" s="36" t="s">
-        <v>52</v>
+      <c r="H45" s="35" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -2841,8 +2859,8 @@
       <c r="G46" s="2">
         <v>0</v>
       </c>
-      <c r="H46" s="36" t="s">
-        <v>53</v>
+      <c r="H46" s="35" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -2867,8 +2885,8 @@
       <c r="G47" s="2">
         <v>0</v>
       </c>
-      <c r="H47" s="36" t="s">
-        <v>47</v>
+      <c r="H47" s="35" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -2893,8 +2911,8 @@
       <c r="G48" s="2">
         <v>0</v>
       </c>
-      <c r="H48" s="36" t="s">
-        <v>48</v>
+      <c r="H48" s="35" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
@@ -2919,8 +2937,8 @@
       <c r="G49" s="2">
         <v>0</v>
       </c>
-      <c r="H49" s="36" t="s">
-        <v>49</v>
+      <c r="H49" s="35" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -2945,8 +2963,8 @@
       <c r="G50" s="2">
         <v>0</v>
       </c>
-      <c r="H50" s="36" t="s">
-        <v>50</v>
+      <c r="H50" s="35" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
@@ -2971,8 +2989,8 @@
       <c r="G51" s="2">
         <v>0</v>
       </c>
-      <c r="H51" s="36" t="s">
-        <v>51</v>
+      <c r="H51" s="35" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -2997,8 +3015,8 @@
       <c r="G52" s="2">
         <v>0</v>
       </c>
-      <c r="H52" s="36" t="s">
-        <v>52</v>
+      <c r="H52" s="35" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -3023,73 +3041,73 @@
       <c r="G53" s="2">
         <v>0</v>
       </c>
-      <c r="H53" s="36" t="s">
-        <v>53</v>
+      <c r="H53" s="35" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="20">
         <v>44664</v>
       </c>
-      <c r="B54" s="36">
-        <v>0</v>
-      </c>
-      <c r="C54" s="36">
-        <v>0</v>
-      </c>
-      <c r="D54" s="36">
-        <v>0</v>
-      </c>
-      <c r="E54" s="36">
-        <v>0</v>
-      </c>
-      <c r="F54" s="36">
-        <v>0</v>
-      </c>
-      <c r="G54" s="36">
-        <v>0</v>
-      </c>
-      <c r="H54" s="36" t="s">
-        <v>47</v>
+      <c r="B54" s="35">
+        <v>0</v>
+      </c>
+      <c r="C54" s="35">
+        <v>0</v>
+      </c>
+      <c r="D54" s="35">
+        <v>0</v>
+      </c>
+      <c r="E54" s="35">
+        <v>0</v>
+      </c>
+      <c r="F54" s="35">
+        <v>0</v>
+      </c>
+      <c r="G54" s="35">
+        <v>0</v>
+      </c>
+      <c r="H54" s="35" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="20">
         <v>44665</v>
       </c>
-      <c r="B55" s="36">
-        <v>0</v>
-      </c>
-      <c r="C55" s="36">
-        <v>0</v>
-      </c>
-      <c r="D55" s="36">
-        <v>0</v>
-      </c>
-      <c r="E55" s="36">
-        <v>0</v>
-      </c>
-      <c r="F55" s="36">
-        <v>0</v>
-      </c>
-      <c r="G55" s="36">
-        <v>0</v>
-      </c>
-      <c r="H55" s="36" t="s">
-        <v>48</v>
+      <c r="B55" s="35">
+        <v>0</v>
+      </c>
+      <c r="C55" s="35">
+        <v>0</v>
+      </c>
+      <c r="D55" s="35">
+        <v>0</v>
+      </c>
+      <c r="E55" s="35">
+        <v>0</v>
+      </c>
+      <c r="F55" s="35">
+        <v>0</v>
+      </c>
+      <c r="G55" s="35">
+        <v>0</v>
+      </c>
+      <c r="H55" s="35" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="20">
         <v>44666</v>
       </c>
-      <c r="B56" s="36">
-        <v>0</v>
-      </c>
-      <c r="C56" s="36">
-        <v>0</v>
-      </c>
-      <c r="D56" s="36">
+      <c r="B56" s="35">
+        <v>0</v>
+      </c>
+      <c r="C56" s="35">
+        <v>0</v>
+      </c>
+      <c r="D56" s="35">
         <v>0</v>
       </c>
       <c r="E56" s="2">
@@ -3098,24 +3116,24 @@
       <c r="F56" s="2">
         <v>0</v>
       </c>
-      <c r="G56" s="36">
-        <v>0</v>
-      </c>
-      <c r="H56" s="36" t="s">
-        <v>49</v>
+      <c r="G56" s="35">
+        <v>0</v>
+      </c>
+      <c r="H56" s="35" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="20">
         <v>44667</v>
       </c>
-      <c r="B57" s="36">
-        <v>0</v>
-      </c>
-      <c r="C57" s="36">
-        <v>0</v>
-      </c>
-      <c r="D57" s="36">
+      <c r="B57" s="35">
+        <v>0</v>
+      </c>
+      <c r="C57" s="35">
+        <v>0</v>
+      </c>
+      <c r="D57" s="35">
         <v>0</v>
       </c>
       <c r="E57" s="2">
@@ -3124,24 +3142,24 @@
       <c r="F57" s="2">
         <v>0</v>
       </c>
-      <c r="G57" s="36">
-        <v>0</v>
-      </c>
-      <c r="H57" s="36" t="s">
-        <v>50</v>
+      <c r="G57" s="35">
+        <v>0</v>
+      </c>
+      <c r="H57" s="35" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="20">
         <v>44668</v>
       </c>
-      <c r="B58" s="36">
-        <v>0</v>
-      </c>
-      <c r="C58" s="36">
-        <v>0</v>
-      </c>
-      <c r="D58" s="36">
+      <c r="B58" s="35">
+        <v>0</v>
+      </c>
+      <c r="C58" s="35">
+        <v>0</v>
+      </c>
+      <c r="D58" s="35">
         <v>0</v>
       </c>
       <c r="E58" s="2">
@@ -3150,24 +3168,24 @@
       <c r="F58" s="2">
         <v>0</v>
       </c>
-      <c r="G58" s="36">
-        <v>0</v>
-      </c>
-      <c r="H58" s="36" t="s">
-        <v>51</v>
+      <c r="G58" s="35">
+        <v>0</v>
+      </c>
+      <c r="H58" s="35" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="20">
         <v>44669</v>
       </c>
-      <c r="B59" s="36">
-        <v>0</v>
-      </c>
-      <c r="C59" s="36">
-        <v>0</v>
-      </c>
-      <c r="D59" s="36">
+      <c r="B59" s="35">
+        <v>0</v>
+      </c>
+      <c r="C59" s="35">
+        <v>0</v>
+      </c>
+      <c r="D59" s="35">
         <v>0</v>
       </c>
       <c r="E59" s="2">
@@ -3176,24 +3194,24 @@
       <c r="F59" s="2">
         <v>0</v>
       </c>
-      <c r="G59" s="36">
-        <v>0</v>
-      </c>
-      <c r="H59" s="36" t="s">
-        <v>52</v>
+      <c r="G59" s="35">
+        <v>0</v>
+      </c>
+      <c r="H59" s="35" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="20">
         <v>44670</v>
       </c>
-      <c r="B60" s="36">
+      <c r="B60" s="35">
         <v>6</v>
       </c>
-      <c r="C60" s="36">
+      <c r="C60" s="35">
         <v>6</v>
       </c>
-      <c r="D60" s="36">
+      <c r="D60" s="35">
         <v>6</v>
       </c>
       <c r="E60" s="2">
@@ -3202,24 +3220,24 @@
       <c r="F60" s="2">
         <v>0</v>
       </c>
-      <c r="G60" s="36">
-        <v>0</v>
-      </c>
-      <c r="H60" s="36" t="s">
-        <v>53</v>
+      <c r="G60" s="35">
+        <v>0</v>
+      </c>
+      <c r="H60" s="35" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="20">
         <v>44671</v>
       </c>
-      <c r="B61" s="36">
-        <v>3</v>
-      </c>
-      <c r="C61" s="36">
-        <v>3</v>
-      </c>
-      <c r="D61" s="36">
+      <c r="B61" s="35">
+        <v>3</v>
+      </c>
+      <c r="C61" s="35">
+        <v>3</v>
+      </c>
+      <c r="D61" s="35">
         <v>3</v>
       </c>
       <c r="E61" s="2">
@@ -3228,24 +3246,24 @@
       <c r="F61" s="2">
         <v>0</v>
       </c>
-      <c r="G61" s="36">
-        <v>0</v>
-      </c>
-      <c r="H61" s="36" t="s">
-        <v>47</v>
+      <c r="G61" s="35">
+        <v>0</v>
+      </c>
+      <c r="H61" s="35" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="20">
         <v>44672</v>
       </c>
-      <c r="B62" s="36">
-        <v>0</v>
-      </c>
-      <c r="C62" s="36">
-        <v>0</v>
-      </c>
-      <c r="D62" s="36">
+      <c r="B62" s="35">
+        <v>0</v>
+      </c>
+      <c r="C62" s="35">
+        <v>0</v>
+      </c>
+      <c r="D62" s="35">
         <v>0</v>
       </c>
       <c r="E62" s="2">
@@ -3254,24 +3272,24 @@
       <c r="F62" s="2">
         <v>0</v>
       </c>
-      <c r="G62" s="36">
-        <v>0</v>
-      </c>
-      <c r="H62" s="36" t="s">
-        <v>48</v>
+      <c r="G62" s="35">
+        <v>0</v>
+      </c>
+      <c r="H62" s="35" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="20">
         <v>44673</v>
       </c>
-      <c r="B63" s="36">
-        <v>0</v>
-      </c>
-      <c r="C63" s="36">
-        <v>0</v>
-      </c>
-      <c r="D63" s="36">
+      <c r="B63" s="35">
+        <v>0</v>
+      </c>
+      <c r="C63" s="35">
+        <v>0</v>
+      </c>
+      <c r="D63" s="35">
         <v>0</v>
       </c>
       <c r="E63" s="2">
@@ -3280,24 +3298,24 @@
       <c r="F63" s="2">
         <v>0</v>
       </c>
-      <c r="G63" s="36">
-        <v>0</v>
-      </c>
-      <c r="H63" s="36" t="s">
-        <v>49</v>
+      <c r="G63" s="35">
+        <v>0</v>
+      </c>
+      <c r="H63" s="35" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="20">
         <v>44674</v>
       </c>
-      <c r="B64" s="36">
-        <v>0</v>
-      </c>
-      <c r="C64" s="36">
-        <v>0</v>
-      </c>
-      <c r="D64" s="36">
+      <c r="B64" s="35">
+        <v>0</v>
+      </c>
+      <c r="C64" s="35">
+        <v>0</v>
+      </c>
+      <c r="D64" s="35">
         <v>0</v>
       </c>
       <c r="E64" s="2">
@@ -3306,24 +3324,24 @@
       <c r="F64" s="2">
         <v>0</v>
       </c>
-      <c r="G64" s="36">
-        <v>0</v>
-      </c>
-      <c r="H64" s="36" t="s">
-        <v>50</v>
+      <c r="G64" s="35">
+        <v>0</v>
+      </c>
+      <c r="H64" s="35" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="20">
         <v>44675</v>
       </c>
-      <c r="B65" s="36">
-        <v>0</v>
-      </c>
-      <c r="C65" s="36">
-        <v>0</v>
-      </c>
-      <c r="D65" s="36">
+      <c r="B65" s="35">
+        <v>0</v>
+      </c>
+      <c r="C65" s="35">
+        <v>0</v>
+      </c>
+      <c r="D65" s="35">
         <v>0</v>
       </c>
       <c r="E65" s="2">
@@ -3332,24 +3350,24 @@
       <c r="F65" s="2">
         <v>0</v>
       </c>
-      <c r="G65" s="36">
-        <v>0</v>
-      </c>
-      <c r="H65" s="36" t="s">
-        <v>51</v>
+      <c r="G65" s="35">
+        <v>0</v>
+      </c>
+      <c r="H65" s="35" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="20">
         <v>44676</v>
       </c>
-      <c r="B66" s="36">
-        <v>3</v>
-      </c>
-      <c r="C66" s="36">
-        <v>3</v>
-      </c>
-      <c r="D66" s="36">
+      <c r="B66" s="35">
+        <v>3</v>
+      </c>
+      <c r="C66" s="35">
+        <v>3</v>
+      </c>
+      <c r="D66" s="35">
         <v>3</v>
       </c>
       <c r="E66" s="2">
@@ -3358,24 +3376,24 @@
       <c r="F66" s="2">
         <v>0</v>
       </c>
-      <c r="G66" s="36">
-        <v>0</v>
-      </c>
-      <c r="H66" s="36" t="s">
-        <v>52</v>
+      <c r="G66" s="35">
+        <v>0</v>
+      </c>
+      <c r="H66" s="35" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="20">
         <v>44677</v>
       </c>
-      <c r="B67" s="36">
+      <c r="B67" s="35">
         <v>7</v>
       </c>
-      <c r="C67" s="36">
+      <c r="C67" s="35">
         <v>7</v>
       </c>
-      <c r="D67" s="36">
+      <c r="D67" s="35">
         <v>5</v>
       </c>
       <c r="E67" s="2">
@@ -3384,24 +3402,24 @@
       <c r="F67" s="2">
         <v>0</v>
       </c>
-      <c r="G67" s="36">
-        <v>0</v>
-      </c>
-      <c r="H67" s="36" t="s">
-        <v>53</v>
+      <c r="G67" s="35">
+        <v>0</v>
+      </c>
+      <c r="H67" s="35" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="20">
         <v>44678</v>
       </c>
-      <c r="B68" s="36">
+      <c r="B68" s="35">
         <v>5</v>
       </c>
-      <c r="C68" s="36">
+      <c r="C68" s="35">
         <v>5</v>
       </c>
-      <c r="D68" s="36">
+      <c r="D68" s="35">
         <v>5</v>
       </c>
       <c r="E68" s="2">
@@ -3410,24 +3428,24 @@
       <c r="F68" s="2">
         <v>0</v>
       </c>
-      <c r="G68" s="36">
-        <v>0</v>
-      </c>
-      <c r="H68" s="36" t="s">
-        <v>47</v>
+      <c r="G68" s="35">
+        <v>0</v>
+      </c>
+      <c r="H68" s="35" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="20">
         <v>44679</v>
       </c>
-      <c r="B69" s="36">
+      <c r="B69" s="35">
         <v>5</v>
       </c>
-      <c r="C69" s="36">
+      <c r="C69" s="35">
         <v>5</v>
       </c>
-      <c r="D69" s="36">
+      <c r="D69" s="35">
         <v>5</v>
       </c>
       <c r="E69" s="2">
@@ -3436,11 +3454,11 @@
       <c r="F69" s="2">
         <v>0</v>
       </c>
-      <c r="G69" s="36">
-        <v>0</v>
-      </c>
-      <c r="H69" s="36" t="s">
-        <v>48</v>
+      <c r="G69" s="35">
+        <v>0</v>
+      </c>
+      <c r="H69" s="35" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
@@ -3462,11 +3480,11 @@
       <c r="F70" s="2">
         <v>0</v>
       </c>
-      <c r="G70" s="36">
-        <v>0</v>
-      </c>
-      <c r="H70" s="36" t="s">
-        <v>49</v>
+      <c r="G70" s="35">
+        <v>0</v>
+      </c>
+      <c r="H70" s="35" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -3485,7 +3503,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3497,31 +3515,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>9</v>
+      <c r="E1" s="25" t="s">
+        <v>8</v>
       </c>
       <c r="F1" s="1"/>
-      <c r="G1" s="26" t="s">
-        <v>9</v>
+      <c r="G1" s="25" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="28">
+        <v>57</v>
+      </c>
+      <c r="B2" s="27">
         <f>49.95</f>
         <v>49.95</v>
       </c>
@@ -3529,39 +3547,39 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="28">
+        <v>65</v>
+      </c>
+      <c r="E2" s="27">
         <v>49.95</v>
       </c>
-      <c r="G2" s="29">
+      <c r="G2" s="28">
         <f>SUM(E2:E26)</f>
         <v>445.53000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="28">
+        <v>58</v>
+      </c>
+      <c r="B3" s="27">
         <v>4.67</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="28">
+        <v>66</v>
+      </c>
+      <c r="E3" s="27">
         <f t="shared" ref="E3:E26" si="0">B3*C3</f>
         <v>4.67</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="28">
+        <v>60</v>
+      </c>
+      <c r="B4" s="27">
         <f>149</f>
         <v>149</v>
       </c>
@@ -3569,18 +3587,18 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" s="28">
+        <v>66</v>
+      </c>
+      <c r="E4" s="27">
         <f t="shared" si="0"/>
         <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="28">
+        <v>59</v>
+      </c>
+      <c r="B5" s="27">
         <f>13.3</f>
         <v>13.3</v>
       </c>
@@ -3588,18 +3606,18 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="28">
+        <v>66</v>
+      </c>
+      <c r="E5" s="27">
         <f t="shared" si="0"/>
         <v>13.3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="28">
+        <v>61</v>
+      </c>
+      <c r="B6" s="27">
         <f>3.95</f>
         <v>3.95</v>
       </c>
@@ -3607,18 +3625,18 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="28">
+        <v>63</v>
+      </c>
+      <c r="E6" s="27">
         <f t="shared" si="0"/>
         <v>3.95</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="28">
+        <v>62</v>
+      </c>
+      <c r="B7" s="27">
         <f>13.99</f>
         <v>13.99</v>
       </c>
@@ -3626,357 +3644,792 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="28">
+        <v>64</v>
+      </c>
+      <c r="E7" s="27">
         <f t="shared" si="0"/>
         <v>13.99</v>
       </c>
-      <c r="G7" s="26" t="s">
-        <v>40</v>
+      <c r="G7" s="25" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="28">
+        <v>70</v>
+      </c>
+      <c r="B8" s="27">
         <v>38.99</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="28">
+        <v>64</v>
+      </c>
+      <c r="E8" s="27">
         <f t="shared" si="0"/>
         <v>38.99</v>
       </c>
-      <c r="G8" s="27" t="s">
-        <v>41</v>
+      <c r="G8" s="26" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="28">
+        <v>71</v>
+      </c>
+      <c r="B9" s="27">
         <v>30</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="28">
+        <v>72</v>
+      </c>
+      <c r="E9" s="27">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="28">
+        <v>75</v>
+      </c>
+      <c r="B10" s="27">
         <v>13</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="28">
+        <v>64</v>
+      </c>
+      <c r="E10" s="27">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="28">
+        <v>74</v>
+      </c>
+      <c r="B11" s="27">
         <v>3.74</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="28">
+        <v>66</v>
+      </c>
+      <c r="E11" s="27">
         <f t="shared" si="0"/>
         <v>3.74</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="28">
+        <v>73</v>
+      </c>
+      <c r="B12" s="27">
         <v>8.7899999999999991</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="28">
+        <v>64</v>
+      </c>
+      <c r="E12" s="27">
         <f t="shared" si="0"/>
         <v>8.7899999999999991</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" s="28">
+        <v>76</v>
+      </c>
+      <c r="B13" s="27">
         <v>25</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="28">
+        <v>66</v>
+      </c>
+      <c r="E13" s="27">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" s="28">
+        <v>77</v>
+      </c>
+      <c r="B14" s="27">
         <v>9.89</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="28">
+        <v>64</v>
+      </c>
+      <c r="E14" s="27">
         <f t="shared" si="0"/>
         <v>9.89</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="28">
+        <v>78</v>
+      </c>
+      <c r="B15" s="27">
         <v>10.79</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="28">
+        <v>64</v>
+      </c>
+      <c r="E15" s="27">
         <f t="shared" si="0"/>
         <v>10.79</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="28">
+        <v>71</v>
+      </c>
+      <c r="B16" s="27">
         <v>30</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="28">
+        <v>79</v>
+      </c>
+      <c r="E16" s="27">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" s="28">
+        <v>80</v>
+      </c>
+      <c r="B17" s="27">
         <v>10.96</v>
       </c>
       <c r="C17" s="2">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="28">
+        <v>81</v>
+      </c>
+      <c r="E17" s="27">
         <f t="shared" si="0"/>
         <v>10.96</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" s="28">
+        <v>82</v>
+      </c>
+      <c r="B18" s="27">
         <v>0.87</v>
       </c>
       <c r="C18" s="2">
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="28">
+        <v>66</v>
+      </c>
+      <c r="E18" s="27">
         <f t="shared" si="0"/>
         <v>2.61</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" s="28">
+        <v>83</v>
+      </c>
+      <c r="B19" s="27">
         <v>7.8E-2</v>
       </c>
       <c r="C19" s="2">
         <v>10</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="28">
+        <v>66</v>
+      </c>
+      <c r="E19" s="27">
         <f t="shared" si="0"/>
         <v>0.78</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B20" s="28">
+        <v>84</v>
+      </c>
+      <c r="B20" s="27">
         <v>0.16700000000000001</v>
       </c>
       <c r="C20" s="2">
         <v>10</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="28">
+        <v>66</v>
+      </c>
+      <c r="E20" s="27">
         <f t="shared" si="0"/>
         <v>1.6700000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B21" s="28">
+        <v>84</v>
+      </c>
+      <c r="B21" s="27">
         <v>0.8</v>
       </c>
       <c r="C21" s="2">
         <v>5</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="28">
+        <v>66</v>
+      </c>
+      <c r="E21" s="27">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="37">
+      <c r="A22" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="36">
         <v>0.11</v>
       </c>
-      <c r="C22" s="36">
+      <c r="C22" s="35">
         <v>10</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="37">
+        <v>66</v>
+      </c>
+      <c r="E22" s="36">
         <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" s="37">
+      <c r="A23" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="36">
         <v>1.93</v>
       </c>
-      <c r="C23" s="36">
+      <c r="C23" s="35">
         <v>5</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="37">
+        <v>66</v>
+      </c>
+      <c r="E23" s="36">
         <f t="shared" si="0"/>
         <v>9.65</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" s="37">
+      <c r="A24" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="36">
         <v>1.96</v>
       </c>
-      <c r="C24" s="36">
+      <c r="C24" s="35">
         <v>3</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E24" s="37">
+        <v>66</v>
+      </c>
+      <c r="E24" s="36">
         <f t="shared" si="0"/>
         <v>5.88</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="37">
+      <c r="A25" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="36">
         <v>0.36199999999999999</v>
       </c>
-      <c r="C25" s="36">
+      <c r="C25" s="35">
         <v>10</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" s="37">
+        <v>66</v>
+      </c>
+      <c r="E25" s="36">
         <f t="shared" si="0"/>
         <v>3.62</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="36">
+        <v>0.02</v>
+      </c>
+      <c r="C26" s="35">
+        <v>10</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="36">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00848B0B-DFE7-4161-B145-050C19D17323}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="27">
+        <f>49.95</f>
+        <v>49.95</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="27">
+        <v>49.95</v>
+      </c>
+      <c r="G2" s="28">
+        <f>SUM(E2:E22)</f>
+        <v>342.04700000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="27">
+        <v>4.67</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="27">
+        <f t="shared" ref="E3:E22" si="0">B3*C3</f>
+        <v>4.67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="27">
+        <f>149</f>
+        <v>149</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="27">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="27">
+        <f>13.3</f>
+        <v>13.3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="27">
+        <f t="shared" si="0"/>
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="27">
+        <f>3.95</f>
+        <v>3.95</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="27">
+        <f t="shared" si="0"/>
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="27">
+        <f>13.99</f>
+        <v>13.99</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="27">
+        <f t="shared" si="0"/>
+        <v>13.99</v>
+      </c>
+      <c r="G7" s="38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="27">
+        <v>3.8</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="27">
+        <f t="shared" si="0"/>
+        <v>3.8</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B26" s="37">
+      <c r="B9" s="27">
+        <v>0.748</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="27">
+        <f t="shared" si="0"/>
+        <v>0.748</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="27">
+        <v>2.637</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="27">
+        <f t="shared" si="0"/>
+        <v>2.637</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="27">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="27">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="27">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="27">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="27">
+        <v>2.1920000000000002</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="27">
+        <f t="shared" si="0"/>
+        <v>2.1920000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="27">
+        <v>0.87</v>
+      </c>
+      <c r="C14" s="2">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="27">
+        <f t="shared" si="0"/>
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="27">
+        <v>7.8E-2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="27">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="27">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="C16" s="2">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="27">
+        <f t="shared" si="0"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="27">
+        <v>0.8</v>
+      </c>
+      <c r="C17" s="2">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="27">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="36">
+        <v>0.11</v>
+      </c>
+      <c r="C18" s="35">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="36">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="36">
+        <v>1.93</v>
+      </c>
+      <c r="C19" s="35">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="36">
+        <f t="shared" si="0"/>
+        <v>9.65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="36">
+        <v>1.96</v>
+      </c>
+      <c r="C20" s="35">
+        <v>3</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="36">
+        <f t="shared" si="0"/>
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="36">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="C21" s="35">
+        <v>10</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="36">
+        <f t="shared" si="0"/>
+        <v>3.62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="36">
         <v>0.02</v>
       </c>
-      <c r="C26" s="36">
+      <c r="C22" s="35">
         <v>10</v>
       </c>
-      <c r="D26" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="37">
+      <c r="D22" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="36">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>

</xml_diff>

<commit_message>
added example budget and notes
</commit_message>
<xml_diff>
--- a/FinalProject/Budget.xlsx
+++ b/FinalProject/Budget.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkans\OneDrive\Desktop\stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\project-lab-1\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9312B5FA-716A-4E2B-A810-EA8D11EF991F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DA22BF-58D2-4EE0-B0EE-0B6CC32C74FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{8BB2A8C5-712E-4190-8588-7F5E0E3A700D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{8BB2A8C5-712E-4190-8588-7F5E0E3A700D}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Budget" sheetId="1" r:id="rId1"/>
     <sheet name="Labor Hours" sheetId="2" r:id="rId2"/>
     <sheet name="Material Costs" sheetId="3" r:id="rId3"/>
-    <sheet name="Bill Of Materials" sheetId="4" r:id="rId4"/>
+    <sheet name="BOM" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="123">
   <si>
     <t>Project Lab 1</t>
   </si>
@@ -309,16 +309,103 @@
     <t xml:space="preserve">Screw terminals </t>
   </si>
   <si>
-    <t>Phototransistors (2)</t>
-  </si>
-  <si>
-    <t>Infrared Sensors (3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCB </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Servo Motors </t>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Price/Unit</t>
+  </si>
+  <si>
+    <t>Basys 3 Board</t>
+  </si>
+  <si>
+    <t>Rover 5 Chasis</t>
+  </si>
+  <si>
+    <t>H-Bridge PCB</t>
+  </si>
+  <si>
+    <t>OSRAM SFH 309 Phototransistors</t>
+  </si>
+  <si>
+    <t>1/4 Watt Resistors</t>
+  </si>
+  <si>
+    <t>Prototype Board</t>
+  </si>
+  <si>
+    <t>Purchased</t>
+  </si>
+  <si>
+    <t>digilent.com</t>
+  </si>
+  <si>
+    <t>pololu.com</t>
+  </si>
+  <si>
+    <t>mouser.com</t>
+  </si>
+  <si>
+    <t>amazon.com</t>
+  </si>
+  <si>
+    <t>Screw Terminals</t>
+  </si>
+  <si>
+    <t>lcsc.com</t>
+  </si>
+  <si>
+    <t>LM393 Comparator</t>
+  </si>
+  <si>
+    <t>KEMET C430C106K3R5TA 10uF Capacitor</t>
+  </si>
+  <si>
+    <t>Vishay K104K10X7RF5UL2 100nF Capacitor</t>
+  </si>
+  <si>
+    <t>LD1117v33 3.3V Regulator</t>
+  </si>
+  <si>
+    <t>L7805 5V Regulator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power PCB </t>
+  </si>
+  <si>
+    <t>1N4148 Diodes</t>
+  </si>
+  <si>
+    <t>SN74LVC1G32MDCKREP OR Gate</t>
+  </si>
+  <si>
+    <t>LM317T Adjustable Regulator</t>
+  </si>
+  <si>
+    <t>9V Battery</t>
+  </si>
+  <si>
+    <t>3D Printed Shell</t>
+  </si>
+  <si>
+    <t>TTU MakerSpace</t>
+  </si>
+  <si>
+    <t>Complete Total</t>
+  </si>
+  <si>
+    <t>Servo</t>
+  </si>
+  <si>
+    <t>HW201 IR Sensors</t>
+  </si>
+  <si>
+    <t>Relays</t>
+  </si>
+  <si>
+    <t>Ribbon Cable</t>
   </si>
 </sst>
 </file>
@@ -522,7 +609,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,12 +654,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -615,7 +697,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -933,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2AB47C0-B6FA-4FC5-84F1-E15593E5DB37}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:K32"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,16 +1030,16 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="42" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
@@ -984,7 +1066,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="7"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="54"/>
+      <c r="I3" s="38"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1019,11 +1101,11 @@
       </c>
       <c r="C5" s="4">
         <f>'Labor Hours'!J2</f>
-        <v>78</v>
+        <v>135</v>
       </c>
       <c r="D5" s="16">
         <f>B5*C5</f>
-        <v>1170</v>
+        <v>2025</v>
       </c>
       <c r="E5" s="6">
         <v>15</v>
@@ -1051,11 +1133,11 @@
       </c>
       <c r="C6" s="4">
         <f>'Labor Hours'!J3</f>
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="D6" s="16">
         <f>B6*C6</f>
-        <v>1050</v>
+        <v>1650</v>
       </c>
       <c r="E6" s="6">
         <v>15</v>
@@ -1077,11 +1159,11 @@
       </c>
       <c r="C7" s="4">
         <f>'Labor Hours'!J4</f>
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D7" s="16">
         <f>B7*C7</f>
-        <v>1020</v>
+        <v>1065</v>
       </c>
       <c r="E7" s="6">
         <v>15</v>
@@ -1112,7 +1194,7 @@
       </c>
       <c r="D9" s="16">
         <f>SUM(D5:D7)</f>
-        <v>3240</v>
+        <v>4740</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="4" t="s">
@@ -1135,7 +1217,7 @@
       </c>
       <c r="D10" s="17">
         <f>D9</f>
-        <v>3240</v>
+        <v>4740</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>15</v>
@@ -1156,7 +1238,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="18">
         <f>SUM(D9:D10)</f>
-        <v>6480</v>
+        <v>9480</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="4"/>
@@ -1164,10 +1246,10 @@
         <f>SUM(G9:G10)</f>
         <v>14400</v>
       </c>
-      <c r="I11" s="44" t="s">
+      <c r="I11" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="44"/>
+      <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
@@ -1176,10 +1258,10 @@
       <c r="E12" s="6"/>
       <c r="F12" s="4"/>
       <c r="G12" s="7"/>
-      <c r="I12" s="45" t="s">
+      <c r="I12" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="46"/>
+      <c r="J12" s="45"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -1191,10 +1273,10 @@
       <c r="E13" s="6"/>
       <c r="F13" s="4"/>
       <c r="G13" s="7"/>
-      <c r="I13" s="47" t="s">
+      <c r="I13" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="48"/>
+      <c r="J13" s="47"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1221,10 +1303,10 @@
         <f>E14*F14</f>
         <v>600</v>
       </c>
-      <c r="I14" s="49" t="s">
+      <c r="I14" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="50"/>
+      <c r="J14" s="49"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1376,14 +1458,14 @@
         <v>28</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="43" t="s">
+      <c r="H23" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43" t="s">
+      <c r="I23" s="42"/>
+      <c r="J23" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="K23" s="43"/>
+      <c r="K23" s="42"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -1398,7 +1480,7 @@
       </c>
       <c r="D24" s="17">
         <f>B24*C24*H24</f>
-        <v>16.199639999999999</v>
+        <v>22.499500000000001</v>
       </c>
       <c r="E24" s="33">
         <v>449.99</v>
@@ -1410,14 +1492,14 @@
         <f>E24*F24*J24</f>
         <v>26.999400000000001</v>
       </c>
-      <c r="H24" s="43">
-        <v>18</v>
-      </c>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43">
+      <c r="H24" s="42">
+        <v>25</v>
+      </c>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42">
         <v>30</v>
       </c>
-      <c r="K24" s="43"/>
+      <c r="K24" s="42"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -1432,7 +1514,7 @@
       </c>
       <c r="D25" s="17">
         <f>B25*C25*H24</f>
-        <v>14.940000000000001</v>
+        <v>20.75</v>
       </c>
       <c r="E25" s="33">
         <v>415</v>
@@ -1458,7 +1540,7 @@
       </c>
       <c r="D26" s="10">
         <f>B26*C26*H24</f>
-        <v>3.59964</v>
+        <v>4.9994999999999994</v>
       </c>
       <c r="E26" s="34">
         <v>99</v>
@@ -1484,7 +1566,7 @@
       </c>
       <c r="D27" s="29">
         <f>B27*C27*H24</f>
-        <v>3.59964</v>
+        <v>4.9994999999999994</v>
       </c>
       <c r="E27" s="32">
         <f>99</f>
@@ -1506,7 +1588,7 @@
       <c r="C28" s="4"/>
       <c r="D28" s="18">
         <f>SUM(D24:D27)</f>
-        <v>38.338920000000002</v>
+        <v>53.248499999999993</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="4"/>
@@ -1531,7 +1613,7 @@
       <c r="C30" s="4"/>
       <c r="D30" s="19">
         <f>SUM(D11,D17,D21,D28)</f>
-        <v>7378.8689199999999</v>
+        <v>10393.7785</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="4"/>
@@ -1550,7 +1632,7 @@
       </c>
       <c r="D31" s="17">
         <f>D30*C31</f>
-        <v>4058.3779060000002</v>
+        <v>5716.5781750000006</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="9">
@@ -1571,7 +1653,7 @@
       </c>
       <c r="D32" s="19">
         <f>SUM(D30:D31)</f>
-        <v>11437.246826000001</v>
+        <v>16110.356675000001</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="15" t="s">
@@ -1605,10 +1687,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7020275-B2DA-4DA8-8538-10FD245A3C38}">
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AA32" sqref="AA32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1638,10 +1720,10 @@
       <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="51"/>
+      <c r="J1" s="50"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="20">
@@ -1672,8 +1754,8 @@
         <v>9</v>
       </c>
       <c r="J2" s="22">
-        <f>SUM(B2:B53)</f>
-        <v>78</v>
+        <f>SUM(B2:B78)</f>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1705,8 +1787,8 @@
         <v>42</v>
       </c>
       <c r="J3" s="22">
-        <f>SUM(C2:C53)</f>
-        <v>70</v>
+        <f>SUM(C2:C78)</f>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1738,8 +1820,8 @@
         <v>43</v>
       </c>
       <c r="J4" s="22">
-        <f>SUM(D2:D53)</f>
-        <v>68</v>
+        <f>SUM(D2:D578)</f>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1786,7 +1868,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -1944,10 +2026,10 @@
       <c r="H11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="52" t="s">
+      <c r="I11" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="43"/>
+      <c r="J11" s="42"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="20">
@@ -1974,10 +2056,10 @@
       <c r="H12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="53" t="s">
+      <c r="I12" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="J12" s="51"/>
+      <c r="J12" s="50"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="20">
@@ -2094,7 +2176,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
@@ -2660,7 +2742,7 @@
         <v>44649</v>
       </c>
       <c r="B39" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C39" s="2">
         <v>3</v>
@@ -2770,7 +2852,7 @@
         <v>0</v>
       </c>
       <c r="D43" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E43" s="2">
         <v>0</v>
@@ -2868,10 +2950,10 @@
         <v>44657</v>
       </c>
       <c r="B47" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D47" s="2">
         <v>3</v>
@@ -3050,13 +3132,13 @@
         <v>44664</v>
       </c>
       <c r="B54" s="35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C54" s="35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D54" s="35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E54" s="35">
         <v>0</v>
@@ -3212,7 +3294,7 @@
         <v>6</v>
       </c>
       <c r="D60" s="35">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E60" s="2">
         <v>0</v>
@@ -3362,13 +3444,13 @@
         <v>44676</v>
       </c>
       <c r="B66" s="35">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C66" s="35">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D66" s="35">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E66" s="2">
         <v>0</v>
@@ -3388,13 +3470,13 @@
         <v>44677</v>
       </c>
       <c r="B67" s="35">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C67" s="35">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D67" s="35">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E67" s="2">
         <v>0</v>
@@ -3414,10 +3496,10 @@
         <v>44678</v>
       </c>
       <c r="B68" s="35">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C68" s="35">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D68" s="35">
         <v>5</v>
@@ -3446,7 +3528,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="35">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E69" s="2">
         <v>0</v>
@@ -3466,13 +3548,13 @@
         <v>44680</v>
       </c>
       <c r="B70" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C70" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D70" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E70" s="2">
         <v>0</v>
@@ -3485,6 +3567,214 @@
       </c>
       <c r="H70" s="35" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="20">
+        <v>44681</v>
+      </c>
+      <c r="B71" s="2">
+        <v>12</v>
+      </c>
+      <c r="C71" s="2">
+        <v>7</v>
+      </c>
+      <c r="D71" s="2">
+        <v>2</v>
+      </c>
+      <c r="E71" s="2">
+        <v>0</v>
+      </c>
+      <c r="F71" s="2">
+        <v>0</v>
+      </c>
+      <c r="G71" s="35">
+        <v>0</v>
+      </c>
+      <c r="H71" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" s="20">
+        <v>44682</v>
+      </c>
+      <c r="B72" s="2">
+        <v>0</v>
+      </c>
+      <c r="C72" s="2">
+        <v>0</v>
+      </c>
+      <c r="D72" s="2">
+        <v>0</v>
+      </c>
+      <c r="E72" s="2">
+        <v>0</v>
+      </c>
+      <c r="F72" s="2">
+        <v>0</v>
+      </c>
+      <c r="G72" s="35">
+        <v>0</v>
+      </c>
+      <c r="H72" s="35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" s="20">
+        <v>44683</v>
+      </c>
+      <c r="B73" s="2">
+        <v>0</v>
+      </c>
+      <c r="C73" s="2">
+        <v>0</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0</v>
+      </c>
+      <c r="E73" s="2">
+        <v>0</v>
+      </c>
+      <c r="F73" s="2">
+        <v>0</v>
+      </c>
+      <c r="G73" s="35">
+        <v>0</v>
+      </c>
+      <c r="H73" s="35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" s="20">
+        <v>44684</v>
+      </c>
+      <c r="B74" s="2">
+        <v>0</v>
+      </c>
+      <c r="C74" s="2">
+        <v>0</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0</v>
+      </c>
+      <c r="E74" s="2">
+        <v>0</v>
+      </c>
+      <c r="F74" s="2">
+        <v>0</v>
+      </c>
+      <c r="G74" s="35">
+        <v>0</v>
+      </c>
+      <c r="H74" s="35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" s="20">
+        <v>44685</v>
+      </c>
+      <c r="B75" s="2">
+        <v>0</v>
+      </c>
+      <c r="C75" s="2">
+        <v>0</v>
+      </c>
+      <c r="D75" s="2">
+        <v>0</v>
+      </c>
+      <c r="E75" s="2">
+        <v>0</v>
+      </c>
+      <c r="F75" s="2">
+        <v>0</v>
+      </c>
+      <c r="G75" s="35">
+        <v>0</v>
+      </c>
+      <c r="H75" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" s="20">
+        <v>44686</v>
+      </c>
+      <c r="B76" s="2">
+        <v>0</v>
+      </c>
+      <c r="C76" s="2">
+        <v>0</v>
+      </c>
+      <c r="D76" s="2">
+        <v>0</v>
+      </c>
+      <c r="E76" s="2">
+        <v>0</v>
+      </c>
+      <c r="F76" s="2">
+        <v>0</v>
+      </c>
+      <c r="G76" s="35">
+        <v>0</v>
+      </c>
+      <c r="H76" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" s="20">
+        <v>44687</v>
+      </c>
+      <c r="B77" s="2">
+        <v>0</v>
+      </c>
+      <c r="C77" s="2">
+        <v>0</v>
+      </c>
+      <c r="D77" s="2">
+        <v>0</v>
+      </c>
+      <c r="E77" s="2">
+        <v>0</v>
+      </c>
+      <c r="F77" s="2">
+        <v>0</v>
+      </c>
+      <c r="G77" s="35">
+        <v>0</v>
+      </c>
+      <c r="H77" s="35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78" s="20">
+        <v>44688</v>
+      </c>
+      <c r="B78" s="2">
+        <v>0</v>
+      </c>
+      <c r="C78" s="2">
+        <v>0</v>
+      </c>
+      <c r="D78" s="2">
+        <v>0</v>
+      </c>
+      <c r="E78" s="2">
+        <v>0</v>
+      </c>
+      <c r="F78" s="2">
+        <v>0</v>
+      </c>
+      <c r="G78" s="35">
+        <v>0</v>
+      </c>
+      <c r="H78" s="35" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -4005,433 +4295,477 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00848B0B-DFE7-4161-B145-050C19D17323}">
-  <dimension ref="A1:G22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216169FD-7E47-4C5A-874F-EDD060A43C54}">
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="38" t="s">
+      <c r="A1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="38" t="s">
-        <v>8</v>
+      <c r="G1" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="27">
-        <f>49.95</f>
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>149.99</v>
+      </c>
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E25" si="0">B2*C2</f>
+        <v>149.99</v>
+      </c>
+      <c r="G2" s="53">
+        <f>ROUND(SUM(E2:E25),2)</f>
+        <v>322.58999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>49.95</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>49.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="27">
-        <v>49.95</v>
-      </c>
-      <c r="G2" s="28">
-        <f>SUM(E2:E22)</f>
-        <v>342.04700000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="27">
-        <v>4.67</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="C4">
+        <v>14.99</v>
+      </c>
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>14.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0.49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>3.6000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="27">
-        <f t="shared" ref="E3:E22" si="0">B3*C3</f>
-        <v>4.67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="27">
-        <f>149</f>
-        <v>149</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="C7">
+        <v>0.41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="27">
+      <c r="C8">
+        <v>29.99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="0"/>
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="27">
-        <f>13.3</f>
+        <v>29.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0.1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0.42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0.8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>0.42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0.83</v>
+      </c>
+      <c r="D14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0.69</v>
+      </c>
+      <c r="D15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0.5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>0.1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1.93</v>
+      </c>
+      <c r="D18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1.93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0.8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>15.99</v>
+      </c>
+      <c r="D20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>15.99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
         <v>13.3</v>
       </c>
-      <c r="C5" s="2">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="27">
+      <c r="D21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21">
         <f t="shared" si="0"/>
-        <v>26.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="27">
-        <f>3.95</f>
-        <v>3.95</v>
-      </c>
-      <c r="C6" s="2">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22">
         <v>1</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="27">
-        <f t="shared" si="0"/>
-        <v>3.95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="27">
-        <f>13.99</f>
-        <v>13.99</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="27">
-        <f t="shared" si="0"/>
-        <v>13.99</v>
-      </c>
-      <c r="G7" s="38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" s="27">
-        <v>3.8</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="27">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="G8" s="39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="27">
-        <v>0.748</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="27">
-        <f t="shared" si="0"/>
-        <v>0.748</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="27">
-        <v>2.637</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="27">
-        <f t="shared" si="0"/>
-        <v>2.637</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="27">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="27">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="27">
+      <c r="C22">
         <v>30</v>
       </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="27">
+      <c r="D22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="27">
-        <v>2.1920000000000002</v>
-      </c>
-      <c r="C13" s="2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>0.88</v>
+      </c>
+      <c r="D23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>2.5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25">
         <v>1</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" s="27">
+      <c r="C25">
+        <v>2.29</v>
+      </c>
+      <c r="D25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25">
         <f t="shared" si="0"/>
-        <v>2.1920000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" s="27">
-        <v>0.87</v>
-      </c>
-      <c r="C14" s="2">
-        <v>3</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="27">
-        <f t="shared" si="0"/>
-        <v>2.61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="27">
-        <v>7.8E-2</v>
-      </c>
-      <c r="C15" s="2">
-        <v>10</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="27">
-        <f t="shared" si="0"/>
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="27">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="C16" s="2">
-        <v>10</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="27">
-        <f t="shared" si="0"/>
-        <v>1.6700000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="27">
-        <v>0.8</v>
-      </c>
-      <c r="C17" s="2">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="27">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" s="36">
-        <v>0.11</v>
-      </c>
-      <c r="C18" s="35">
-        <v>10</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="36">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" s="36">
-        <v>1.93</v>
-      </c>
-      <c r="C19" s="35">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="36">
-        <f t="shared" si="0"/>
-        <v>9.65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" s="36">
-        <v>1.96</v>
-      </c>
-      <c r="C20" s="35">
-        <v>3</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="36">
-        <f t="shared" si="0"/>
-        <v>5.88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" s="36">
-        <v>0.36199999999999999</v>
-      </c>
-      <c r="C21" s="35">
-        <v>10</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="36">
-        <f t="shared" si="0"/>
-        <v>3.62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="B22" s="36">
-        <v>0.02</v>
-      </c>
-      <c r="C22" s="35">
-        <v>10</v>
-      </c>
-      <c r="D22" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="36">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>2.29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>